<commit_message>
WIP idle animation system.
</commit_message>
<xml_diff>
--- a/Source/IdleMovementAnimPlan.xlsx
+++ b/Source/IdleMovementAnimPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\steamapps\common\RimWorld\Mods\AdvancedAnimationMod\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E261B285-833F-46D8-8FBE-FBCBFE65AFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB81C11-7AB2-4B5E-9DBC-B5122EF6526A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F5F83987-0049-4054-8FEB-C8C7224BCC9C}"/>
   </bookViews>
@@ -47,12 +47,6 @@
     <t>Medium sharp/stab</t>
   </si>
   <si>
-    <t>Huge sharp/stab</t>
-  </si>
-  <si>
-    <t>Huge blunt</t>
-  </si>
-  <si>
     <t>Knives, daggers,
 hatchets</t>
   </si>
@@ -64,13 +58,6 @@
     <t>Most swords</t>
   </si>
   <si>
-    <t>Huge swords,
-huge lances/spears</t>
-  </si>
-  <si>
-    <t>Huge hammers</t>
-  </si>
-  <si>
     <t>Idle</t>
   </si>
   <si>
@@ -87,13 +74,26 @@
   </si>
   <si>
     <t>Move Vertical</t>
+  </si>
+  <si>
+    <t>Colossal sharp/stab</t>
+  </si>
+  <si>
+    <t>Colossal blunt</t>
+  </si>
+  <si>
+    <t>Colossal swords,
+Colossal lances/spears</t>
+  </si>
+  <si>
+    <t>Colossal hammers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +123,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +151,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -221,13 +233,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -250,10 +263,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
@@ -570,7 +587,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,53 +607,53 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="42.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -646,7 +663,7 @@
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -656,7 +673,7 @@
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -666,7 +683,7 @@
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>

</xml_diff>